<commit_message>
3rd Training Data Set Created
</commit_message>
<xml_diff>
--- a/2009.xlsx
+++ b/2009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NMath\Desktop\keras\Data-Analysis-Project-2022-T20-World-Cup-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AA8EB9-C3D7-4DDB-A0ED-8F88786B22E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1840466-984D-48DC-8808-0B0447E9A95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3648" yWindow="1644" windowWidth="15576" windowHeight="8076" xr2:uid="{89CAEAF6-D4C8-41C3-911E-1B738DC56D45}"/>
   </bookViews>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CB5153-1144-43C3-B390-96244B498E21}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>